<commit_message>
IMPROVE: Balance of Payment Ids
</commit_message>
<xml_diff>
--- a/files/balanceOfPayment/balanca-de-pagamento.xlsx
+++ b/files/balanceOfPayment/balanca-de-pagamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arlindo Boa\Desktop\tactic\files\balanceOfPayment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67974568-C4EA-42A9-9491-2D153071089D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421EF0F4-5DDD-49FE-976F-9FC03C7695C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B0C785E8-75DE-4CFD-AE1E-D05EFF457645}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Importação</t>
   </si>
   <si>
-    <t>serviços</t>
-  </si>
-  <si>
     <t>Rendimentos Primários</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
       </rPr>
       <t>ébito</t>
     </r>
+  </si>
+  <si>
+    <t>Serviços</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +568,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -765,7 +765,7 @@
     </row>
     <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="14"/>
@@ -789,7 +789,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5">
         <v>341.9</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6">
         <v>648.6</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="9" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -925,7 +925,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="6">
         <v>98.9</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6">
         <v>458.8</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="6">
         <v>479</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="6">
         <v>76</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="6">
         <v>95.2</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="6">
         <v>187.9</v>

</xml_diff>

<commit_message>
IMPROVE: Exchange Rates Extractor
</commit_message>
<xml_diff>
--- a/files/balanceOfPayment/balanca-de-pagamento.xlsx
+++ b/files/balanceOfPayment/balanca-de-pagamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arlindo Boa\Desktop\tactic\files\balanceOfPayment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421EF0F4-5DDD-49FE-976F-9FC03C7695C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F335F627-45DE-4C03-AE80-C4A7A852A42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B0C785E8-75DE-4CFD-AE1E-D05EFF457645}"/>
   </bookViews>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CFE5A2-4529-4504-8F3D-9069492F1C7A}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>